<commit_message>
updated to add Region for Networking
</commit_message>
<xml_diff>
--- a/oci_tenancy/2.SetUpOCI_Via_TF_v2.0/example/CD3-template.xlsx
+++ b/oci_tenancy/2.SetUpOCI_Via_TF_v2.0/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="204">
   <si>
     <t>Regional</t>
   </si>
@@ -790,10 +790,31 @@
     <t># VCN names should be unique and are case-sensitie across sheets; All fields are mandatory for each VCN except dns_label for which the default value is vcn_name truncated to 15 chars</t>
   </si>
   <si>
-    <t># subnet names are unique and case-sensitive across sheets; All fields are mandatory for each subnet except dns_label for which the default value is subnet_name truncated to 15 chars</t>
-  </si>
-  <si>
     <t># DHCP option is created in the same compartment as the VCN; Whichever DHCP option name(case-sensitie) you have mentioned in the Subnets Sheet should be defined here in this sheet;  if server_type is CustomDnsServer then you should not leave custom_dns_server column empty</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Ashburn</t>
+  </si>
+  <si>
+    <t>Phoenix</t>
+  </si>
+  <si>
+    <t>ASHVCN</t>
+  </si>
+  <si>
+    <t>10.218.255.0/24</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>ashvcn</t>
+  </si>
+  <si>
+    <t># subnet names are unique and case-sensitive across sheets; All fields are mandatory for each subnet except dns_label for which the default value is subnet_name truncated to 15 chars; dhcp_option_name field if left blank means subnet will use default dhcp options of the vcn</t>
   </si>
 </sst>
 </file>
@@ -1906,10 +1927,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1918,11 +1939,12 @@
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="86.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="19" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
         <v>192</v>
       </c>
@@ -1931,8 +1953,9 @@
       <c r="D1" s="27"/>
       <c r="E1" s="27"/>
       <c r="F1" s="27"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="27"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>125</v>
       </c>
@@ -1945,14 +1968,17 @@
       <c r="D2" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="F2" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="G2" s="22" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>67</v>
       </c>
@@ -1967,8 +1993,9 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1983,8 +2010,9 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>100</v>
       </c>
@@ -1993,10 +2021,11 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2005,10 +2034,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:N1"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2022,11 +2051,12 @@
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" style="19" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
         <v>193</v>
       </c>
@@ -2043,8 +2073,9 @@
       <c r="L1" s="27"/>
       <c r="M1" s="27"/>
       <c r="N1" s="27"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="27"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>131</v>
       </c>
@@ -2081,14 +2112,17 @@
       <c r="L2" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="M2" s="22" t="s">
+      <c r="M2" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="N2" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="N2" s="22" t="s">
+      <c r="O2" s="22" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -2117,8 +2151,9 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>100</v>
       </c>
@@ -2135,8 +2170,9 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>101</v>
       </c>
@@ -2153,8 +2189,9 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2169,10 +2206,11 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2181,10 +2219,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2193,11 +2231,12 @@
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="19" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>125</v>
       </c>
@@ -2210,10 +2249,13 @@
       <c r="D1" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="F1" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="22" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2225,10 +2267,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2236,11 +2278,12 @@
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="19"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>131</v>
       </c>
@@ -2277,10 +2320,13 @@
       <c r="L1" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="M1" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="N1" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="N1" s="22" t="s">
+      <c r="O1" s="22" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2494,28 +2540,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="19"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>194</v>
       </c>
@@ -2529,132 +2576,181 @@
       <c r="I1" s="30"/>
       <c r="J1" s="30"/>
       <c r="K1" s="30"/>
-      <c r="L1" s="31"/>
-    </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L1" s="30"/>
+      <c r="M1" s="31"/>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>4</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>100</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>30</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>2</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>100</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="I5" s="3">
+        <v>2</v>
+      </c>
+      <c r="J5" s="3">
+        <v>100</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -2666,11 +2762,11 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
-    </row>
-    <row r="16" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
+      <c r="M15" s="3"/>
+    </row>
+    <row r="16" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -2682,10 +2778,11 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2807,7 +2904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
@@ -2828,7 +2925,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -2976,7 +3073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
@@ -2991,7 +3088,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>

</xml_diff>

<commit_message>
updated Instances and Block Volumes to have region
</commit_message>
<xml_diff>
--- a/oci_tenancy/2.SetUpOCI_Via_TF_v2.0/example/CD3-template.xlsx
+++ b/oci_tenancy/2.SetUpOCI_Via_TF_v2.0/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="202">
   <si>
     <t>Regional</t>
   </si>
@@ -37,9 +37,6 @@
     <t>private</t>
   </si>
   <si>
-    <t>10.110.255.224/28</t>
-  </si>
-  <si>
     <t>vcn_name</t>
   </si>
   <si>
@@ -79,15 +76,9 @@
     <t>type(private|public)</t>
   </si>
   <si>
-    <t>OCPVQLGISAPP01_disk2</t>
-  </si>
-  <si>
     <t>AD1</t>
   </si>
   <si>
-    <t>OCPVQLGISAPP01</t>
-  </si>
-  <si>
     <t>iscsi</t>
   </si>
   <si>
@@ -116,9 +107,6 @@
   </si>
   <si>
     <t>PHXHub-VCN</t>
-  </si>
-  <si>
-    <t>10.110.255.0/24</t>
   </si>
   <si>
     <t>y</t>
@@ -815,6 +803,12 @@
   </si>
   <si>
     <t># subnet names are unique and case-sensitive across sheets; All fields are mandatory for each subnet except dns_label for which the default value is subnet_name truncated to 15 chars; dhcp_option_name field if left blank means subnet will use default dhcp options of the vcn</t>
+  </si>
+  <si>
+    <t>10.110.13.0/24</t>
+  </si>
+  <si>
+    <t>10.110.0.0/16</t>
   </si>
 </sst>
 </file>
@@ -1042,7 +1036,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1102,6 +1095,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1422,74 +1418,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
+      <c r="A1" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C8" s="1"/>
     </row>
@@ -1523,217 +1519,217 @@
     <col min="5" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="19" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>166</v>
-      </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
+    <row r="1" spans="1:6" s="18" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
-        <v>146</v>
+      <c r="A2" s="18" t="s">
+        <v>142</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="D3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="E3" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="B3" s="36" t="s">
+      <c r="F3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="9" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="38"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="9" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="38"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E5" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>68</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="37"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="10"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="39"/>
-      <c r="B7" s="37"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="12"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
-      <c r="B8" s="37"/>
+      <c r="A8" s="38"/>
+      <c r="B8" s="36"/>
       <c r="C8" s="12"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="39"/>
-      <c r="B9" s="37"/>
+      <c r="A9" s="38"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="12"/>
       <c r="D9" s="1"/>
       <c r="E9" s="11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="39"/>
-      <c r="B10" s="37"/>
+      <c r="A10" s="38"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="12"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
-      <c r="B11" s="37"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="12"/>
       <c r="D11" s="1"/>
       <c r="E11" s="11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="37"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="36"/>
       <c r="C12" s="12"/>
       <c r="D12" s="1"/>
       <c r="E12" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
-      <c r="B13" s="37"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="12"/>
       <c r="D13" s="1"/>
       <c r="E13" s="11" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
-      <c r="B14" s="37"/>
+      <c r="A14" s="38"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="12"/>
       <c r="D14" s="1"/>
       <c r="E14" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="39"/>
-      <c r="B15" s="37"/>
+      <c r="A15" s="38"/>
+      <c r="B15" s="36"/>
       <c r="C15" s="10"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
-      <c r="B16" s="37"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="36"/>
       <c r="C16" s="10"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
-      <c r="B17" s="37"/>
+      <c r="A17" s="38"/>
+      <c r="B17" s="36"/>
       <c r="C17" s="10"/>
       <c r="D17" s="1"/>
       <c r="E17" s="11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="39"/>
-      <c r="B18" s="38"/>
+      <c r="A18" s="38"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="10"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F18" s="1"/>
     </row>
@@ -1757,84 +1753,95 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="18"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="19" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" s="18" t="s">
+    <row r="1" spans="1:6" s="18" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="C3" s="17" t="s">
+      <c r="C4" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="E4" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="D3" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>154</v>
+      <c r="F4" s="16" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1842,84 +1849,95 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="18"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="19" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>175</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="B3" s="19" t="s">
+    <row r="1" spans="1:6" s="18" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E3" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="D3" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="E3" s="19" t="s">
+      <c r="F3" s="18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="E4" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="D4" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>154</v>
+      <c r="F4" s="18" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1939,57 +1957,57 @@
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="86.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="19" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="18" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
-        <v>192</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="A1" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>117</v>
+        <v>192</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -1997,16 +2015,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -2014,7 +2032,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2051,92 +2069,92 @@
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" style="19" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" style="18" customWidth="1"/>
     <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
-        <v>193</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
+      <c r="A1" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="G2" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="H2" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="I2" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="J2" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="K2" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="L2" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="I2" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>142</v>
-      </c>
       <c r="M2" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="N2" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="O2" s="22" t="s">
-        <v>117</v>
+        <v>192</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D3" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -2155,7 +2173,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2174,7 +2192,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2231,32 +2249,32 @@
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="19" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="18" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>117</v>
+        <v>192</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2278,56 +2296,56 @@
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="19"/>
+    <col min="13" max="13" width="9.140625" style="18"/>
     <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="I1" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>142</v>
-      </c>
       <c r="M1" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="N1" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="O1" s="22" t="s">
-        <v>117</v>
+        <v>192</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2350,50 +2368,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="B1" s="26"/>
+      <c r="A1" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="25"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B7" s="1"/>
     </row>
@@ -2424,50 +2442,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>118</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
+      <c r="A1" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -2476,13 +2494,13 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2495,22 +2513,22 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2518,16 +2536,16 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2543,12 +2561,12 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="19"/>
+    <col min="1" max="1" width="9.140625" style="18"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
@@ -2563,87 +2581,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>194</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="31"/>
+      <c r="A1" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="30"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="L2" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="I3" s="1">
         <v>4</v>
@@ -2652,39 +2670,39 @@
         <v>100</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I4" s="1">
         <v>2</v>
@@ -2693,37 +2711,37 @@
         <v>100</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>201</v>
       </c>
       <c r="I5" s="3">
         <v>2</v>
@@ -2732,13 +2750,13 @@
         <v>100</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2799,95 +2817,95 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" style="19" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="19"/>
+    <col min="1" max="1" width="32.28515625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" style="18" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>190</v>
-      </c>
-      <c r="B1" s="33"/>
+      <c r="A1" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="32"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>30</v>
+      <c r="A8" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>30</v>
+      <c r="A9" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
-        <v>191</v>
-      </c>
-      <c r="B10" s="35"/>
+      <c r="A10" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="B10" s="34"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -2904,8 +2922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2924,67 +2942,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>203</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
+      <c r="A1" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
     </row>
     <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>51</v>
-      </c>
       <c r="K2" s="15" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
@@ -2993,19 +3011,19 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="21" t="s">
-        <v>162</v>
+        <v>27</v>
+      </c>
+      <c r="K3" s="20" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -3087,60 +3105,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>195</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="A1" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
     </row>
     <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -3154,115 +3172,122 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" customWidth="1"/>
-    <col min="10" max="10" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="18"/>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" customWidth="1"/>
+    <col min="11" max="11" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>165</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="30"/>
+    </row>
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="G2" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="H2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="J2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+        <v>91</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -3273,13 +3298,14 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="4"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C6" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3287,106 +3313,120 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="H2" sqref="H2:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="18"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="19" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>164</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-    </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="18" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+    </row>
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" s="1">
+        <v>302</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="G2" s="15" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="1">
-        <v>302</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated Networking to add support for multiple hub-spoke VCNs updated tagging and backup to include region
</commit_message>
<xml_diff>
--- a/oci_tenancy/2.SetUpOCI_Via_TF_v2.0/example/CD3-template.xlsx
+++ b/oci_tenancy/2.SetUpOCI_Via_TF_v2.0/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="7" r:id="rId1"/>
@@ -599,11 +599,6 @@
     <t>VCN3</t>
   </si>
   <si>
-    <t>VCN Peering
-comma seperated VCNs on right column are peered with VCN on left column
-LPGs and rules are created based on this section</t>
-  </si>
-  <si>
     <t># Rows after &lt;END&gt; or &lt;end&gt; will not be processed; While adding more rules, you should move previous ones to the below and insert new
  rows at the beginning and Enter &lt;END&gt; so that old rules already added don’t get added again;
 This sheet will only add new rules to the route tables; 'RouteRulesinOCI' sheet would be used for overwrite of all route rules in OCI; That means whatever is there in that sheet would be updated as it is in OCI
@@ -618,9 +613,6 @@
     <t># VCN names should be unique and are case-sensitie across sheets; All fields are mandatory for each VCN except dns_label for which the default value is vcn_name truncated to 15 chars</t>
   </si>
   <si>
-    <t># DHCP option is created in the same compartment as the VCN; Whichever DHCP option name(case-sensitie) you have mentioned in the Subnets Sheet should be defined here in this sheet;  if server_type is CustomDnsServer then you should not leave custom_dns_server column empty</t>
-  </si>
-  <si>
     <t>Region</t>
   </si>
   <si>
@@ -640,9 +632,6 @@
   </si>
   <si>
     <t>ashvcn</t>
-  </si>
-  <si>
-    <t># subnet names are unique and case-sensitive across sheets; All fields are mandatory for each subnet except dns_label for which the default value is subnet_name truncated to 15 chars; dhcp_option_name field if left blank means subnet will use default dhcp options of the vcn</t>
   </si>
   <si>
     <t>10.110.13.0/24</t>
@@ -809,6 +798,19 @@
       <t xml:space="preserve"> represents whether you want to add Ping rules for peered VCNs; useful for network related testing
 </t>
     </r>
+  </si>
+  <si>
+    <t># DHCP option is created in the same compartment as the VCN; Whichever DHCP option name(case-sensitie) you have mentioned in the Subnets Sheet should be defined here in this sheet; server_type field is also case-sensitive.  if server_type is CustomDnsServer then you should not leave custom_dns_server column empty</t>
+  </si>
+  <si>
+    <t>VCN Peering
+comma seperated VCNs on right column are peered with VCN on left column
+LPGs and rules are created based on this section; 
+eg: Mention Hub VCN name on left side and all spoke VCN names peered with it on right side</t>
+  </si>
+  <si>
+    <t># subnet names are unique and case-sensitive across sheets; All fields are mandatory for each subnet except dns_label for which the default value is subnet_name truncated to 15 chars; dhcp_option_name field if left blank means subnet will use default dhcp options of the vcn
+vcn_name should be as is as enterd in VCNs sheet</t>
   </si>
 </sst>
 </file>
@@ -1781,7 +1783,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>77</v>
@@ -1801,7 +1803,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>148</v>
@@ -1821,7 +1823,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>151</v>
@@ -1877,7 +1879,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>152</v>
@@ -1897,7 +1899,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>153</v>
@@ -1917,7 +1919,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>154</v>
@@ -1964,7 +1966,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -1987,7 +1989,7 @@
         <v>120</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F2" s="21" t="s">
         <v>159</v>
@@ -2076,7 +2078,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -2131,7 +2133,7 @@
         <v>138</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="N2" s="21" t="s">
         <v>159</v>
@@ -2268,7 +2270,7 @@
         <v>120</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F1" s="21" t="s">
         <v>159</v>
@@ -2339,7 +2341,7 @@
         <v>138</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="N1" s="21" t="s">
         <v>159</v>
@@ -2582,7 +2584,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -2599,7 +2601,7 @@
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -2640,13 +2642,13 @@
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>26</v>
@@ -2681,7 +2683,7 @@
     </row>
     <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>30</v>
@@ -2720,13 +2722,13 @@
     </row>
     <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>194</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>26</v>
@@ -2741,7 +2743,7 @@
         <v>26</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I5" s="3">
         <v>2</v>
@@ -2756,7 +2758,7 @@
         <v>89</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2811,8 +2813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2824,7 +2826,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B1" s="32"/>
     </row>
@@ -2886,9 +2888,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="B10" s="34"/>
     </row>
@@ -2922,8 +2924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2943,7 +2945,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -3002,7 +3004,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
@@ -3106,7 +3108,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -3213,7 +3215,7 @@
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>77</v>
@@ -3251,7 +3253,7 @@
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>148</v>
@@ -3344,7 +3346,7 @@
     </row>
     <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>37</v>
@@ -3370,7 +3372,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>153</v>

</xml_diff>

<commit_message>
updated <END> tags for Neworking Changed columns names order for SecRules and RouteRules Modified fetchCompartmens to accept outdir name
</commit_message>
<xml_diff>
--- a/oci_tenancy/2.SetUpOCI_Via_TF_v2.0/example/CD3-template.xlsx
+++ b/oci_tenancy/2.SetUpOCI_Via_TF_v2.0/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="13"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="208">
   <si>
     <t>Regional</t>
   </si>
@@ -908,7 +908,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -982,17 +982,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -1029,7 +1018,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1066,8 +1055,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1080,13 +1071,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1095,10 +1086,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1117,9 +1108,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1440,11 +1428,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -1542,14 +1530,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="18" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="42" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
@@ -1572,10 +1560,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="38" t="s">
         <v>53</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -1592,8 +1580,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
-      <c r="B4" s="37"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="9" t="s">
         <v>58</v>
       </c>
@@ -1608,8 +1596,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="37"/>
+      <c r="A5" s="41"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="10" t="s">
         <v>163</v>
       </c>
@@ -1624,8 +1612,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="37"/>
+      <c r="A6" s="41"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="10"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
@@ -1636,8 +1624,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="39"/>
-      <c r="B7" s="37"/>
+      <c r="A7" s="41"/>
+      <c r="B7" s="39"/>
       <c r="C7" s="12"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
@@ -1646,8 +1634,8 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
-      <c r="B8" s="37"/>
+      <c r="A8" s="41"/>
+      <c r="B8" s="39"/>
       <c r="C8" s="12"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
@@ -1656,8 +1644,8 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="39"/>
-      <c r="B9" s="37"/>
+      <c r="A9" s="41"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="12"/>
       <c r="D9" s="1"/>
       <c r="E9" s="11" t="s">
@@ -1666,8 +1654,8 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="39"/>
-      <c r="B10" s="37"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="39"/>
       <c r="C10" s="12"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
@@ -1676,8 +1664,8 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
-      <c r="B11" s="37"/>
+      <c r="A11" s="41"/>
+      <c r="B11" s="39"/>
       <c r="C11" s="12"/>
       <c r="D11" s="1"/>
       <c r="E11" s="11" t="s">
@@ -1686,8 +1674,8 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="37"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="39"/>
       <c r="C12" s="12"/>
       <c r="D12" s="1"/>
       <c r="E12" s="11" t="s">
@@ -1696,8 +1684,8 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
-      <c r="B13" s="37"/>
+      <c r="A13" s="41"/>
+      <c r="B13" s="39"/>
       <c r="C13" s="12"/>
       <c r="D13" s="1"/>
       <c r="E13" s="11" t="s">
@@ -1706,8 +1694,8 @@
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
-      <c r="B14" s="37"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="39"/>
       <c r="C14" s="12"/>
       <c r="D14" s="1"/>
       <c r="E14" s="11" t="s">
@@ -1716,8 +1704,8 @@
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="39"/>
-      <c r="B15" s="37"/>
+      <c r="A15" s="41"/>
+      <c r="B15" s="39"/>
       <c r="C15" s="10"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
@@ -1726,8 +1714,8 @@
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
-      <c r="B16" s="37"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="10"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
@@ -1736,8 +1724,8 @@
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
-      <c r="B17" s="37"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="39"/>
       <c r="C17" s="10"/>
       <c r="D17" s="1"/>
       <c r="E17" s="11" t="s">
@@ -1746,8 +1734,8 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="39"/>
-      <c r="B18" s="38"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
@@ -1792,14 +1780,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="18" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1888,14 +1876,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="18" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="37" t="s">
         <v>171</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1967,92 +1955,111 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="86.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="18" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="18"/>
+    <col min="2" max="2" width="11.7109375" style="18" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="18"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="86.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" style="18" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:10" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="E2" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="G2" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="13"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>96</v>
       </c>
@@ -2062,6 +2069,9 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2076,142 +2086,146 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" style="18" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="18"/>
+    <col min="2" max="2" width="11.7109375" style="18" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="18"/>
+    <col min="4" max="4" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="E2" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="G2" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="H2" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="I2" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="J2" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="K2" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="L2" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="M2" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="N2" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="O2" s="13" t="s">
         <v>138</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="N2" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="O2" s="21" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D3" s="1" t="b">
+      <c r="G3" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1">
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1">
         <v>123</v>
       </c>
-      <c r="J3" s="1">
+      <c r="M3" s="1">
         <v>123</v>
       </c>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="D4" s="1" t="b">
+      <c r="G4" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -2221,27 +2235,29 @@
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="D5" s="1" t="b">
+      <c r="G5" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
-        <v>207</v>
-      </c>
+      <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="K5" s="1" t="s">
+        <v>207</v>
+      </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -2251,8 +2267,6 @@
       <c r="A6" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -2267,11 +2281,6 @@
       <c r="O6" s="1"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -2286,9 +2295,6 @@
       <c r="O7" s="1"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -2313,45 +2319,51 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="H1" sqref="H1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="18" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="18"/>
+    <col min="2" max="2" width="19.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" style="18" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>113</v>
-      </c>
+      <c r="H1" s="13"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2361,68 +2373,104 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="18"/>
-    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="18"/>
+    <col min="2" max="2" width="11.7109375" style="18" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="18"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="18"/>
+    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="M1" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="M1" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="O1" s="21" t="s">
-        <v>113</v>
-      </c>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2444,10 +2492,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -2518,14 +2566,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -2636,8 +2684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2657,21 +2705,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="32"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -2835,7 +2883,11 @@
         <v>194</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
     <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2899,10 +2951,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="181.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="33" t="s">
         <v>197</v>
       </c>
-      <c r="B1" s="32"/>
+      <c r="B1" s="34"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -2963,10 +3015,10 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="B10" s="34"/>
+      <c r="B10" s="36"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -2999,7 +3051,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3018,19 +3070,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
     </row>
     <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3103,7 +3155,9 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -3165,10 +3219,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3181,13 +3235,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>198</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3235,6 +3289,11 @@
       </c>
       <c r="D4" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -3272,20 +3331,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="32"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -3407,16 +3466,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="18" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
     </row>
     <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">

</xml_diff>

<commit_message>
updated export route tables to display destination objetc name instead of ocid updated COmpartments, Groups, Policies to hae region coulmn
</commit_message>
<xml_diff>
--- a/oci_tenancy/2.SetUpOCI_Via_TF_v2.0/example/CD3-template.xlsx
+++ b/oci_tenancy/2.SetUpOCI_Via_TF_v2.0/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="208">
   <si>
     <t>Regional</t>
   </si>
@@ -346,10 +346,6 @@
     <t>VM_Admins</t>
   </si>
   <si>
-    <t># Rows after &lt;END&gt; or &lt;end&gt; will not be processed;
-Group Name is mandatory field</t>
-  </si>
-  <si>
     <t>Policy Statements</t>
   </si>
   <si>
@@ -380,10 +376,6 @@
     <t>Compartment Name</t>
   </si>
   <si>
-    <t>$ and * in PolicyStatements would be replaced by PolicyStatementGroup and PolicyStatementCompartment respectively;
-# Rows after &lt;END&gt; or &lt;end&gt; will not be processed;</t>
-  </si>
-  <si>
     <t>PolicyStatementGroups</t>
   </si>
   <si>
@@ -589,12 +581,6 @@
   </si>
   <si>
     <t>VCN3</t>
-  </si>
-  <si>
-    <t># Rows after &lt;END&gt; or &lt;end&gt; will not be processed; While adding more rules, you should move previous ones to the below and insert new
- rows at the beginning and Enter &lt;END&gt; so that old rules already added don’t get added again;
-This sheet will only add new rules to the route tables; 'RouteRulesinOCI' sheet would be used for overwrite of all route rules in OCI; That means whatever is there in that sheet would be updated as it is in OCI
-VCN Name and Compartment Name fields in this sheet are just for informational purpose right now; would be used in future when we allow same subnet names across VCNs</t>
   </si>
   <si>
     <t>Region</t>
@@ -817,25 +803,41 @@
     <t>10.20.30.40/32</t>
   </si>
   <si>
+    <t># Horizontal row specifies the TagNameSpace Names to be created; Vertical row under each TagNameSpace represnts Keys in that tagnamespace; Enter compartment name in which  all tagnamespaces and keys will be created;
+tags get created in Home Region so gie appropriate outdir while execution</t>
+  </si>
+  <si>
+    <t># Rows after &lt;END&gt; or &lt;end&gt; will not be processed; While adding more rules, you should move previous ones to the below and insert new
+ rows at the beginning and Enter &lt;END&gt; so that old rules already added don’t get added again;
+This sheet will only add new rules to the route tables; 'RouteRulesinOCI' sheet would be used for overwrite of all route rules in OCI; That means whatever is there in that sheet would be updated as it is in OCI
+VCN Name and Compartment Name fields in this sheet are just for informational purpose right now; would be used in future when we allow same subnet names across VCNs
+Enter Route Destination Object as either the OCID of component or  the name of component- &lt;vcn_name&gt;_igw|&lt;vcn_name&gt;_lpg|&lt;vcn_name&gt;|ngw|&lt;vcn_name&gt;|drg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># VCN names should be unique and are case-sensitie across sheets; All fields are mandatory for each VCN except dns_label for which the default value is vcn_name truncated to 15 chars
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># subnet names are unique and case-sensitive across sheets; All fields are mandatory for each subnet except dns_label for which the default value is subnet_name truncated to 15 chars; dhcp_option_name field if left blank means subnet will use default dhcp options of the vcn
+vcn_name should be same as enterd in VCNs sheet;
+Route Rules for IGW, NGW and SGW would be created based on parameter values: configure_igw, configure_ngw and configure_sgw respectively for each subnet. The condition is the respectove component should hae been created for that using parameters: igw_required, ngw_required and sgw_required parameters in VCNs sheet.
+</t>
+  </si>
+  <si>
     <t># Leave Parent Compartment empty or mention root if it is under root;
 Rows after &lt;END&gt; or &lt;end&gt; will not be processed;
 Compartment Name is mandatory field
-Compartments, Groups, Policies will be created in Home Region So while executing setUpOCI, choose correct out dir as per your home region</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># VCN names should be unique and are case-sensitie across sheets; All fields are mandatory for each VCN except dns_label for which the default value is vcn_name truncated to 15 chars
-Don’t leave blank lines in between
-</t>
-  </si>
-  <si>
-    <t># subnet names are unique and case-sensitive across sheets; All fields are mandatory for each subnet except dns_label for which the default value is subnet_name truncated to 15 chars; dhcp_option_name field if left blank means subnet will use default dhcp options of the vcn
-vcn_name should be same as enterd in VCNs sheet;
-Route Rules for IGW, NGW and SGW would be created based on parameter values: configure_igw, configure_ngw and configure_sgw respectively for each subnet. The condition is the respectove component should hae been created for that using parameters: igw_required, ngw_required and sgw_required parameters in VCNs sheet.
-Don’t leave blank lines in between</t>
-  </si>
-  <si>
-    <t># Horizontal row specifies the TagNameSpace Names to be created; Vertical row under each TagNameSpace represnts Keys in that tagnamespace; Enter compartment name in which  all tagnamespaces and keys will be created;
-tags get created in Home Region so gie appropriate outdir while execution</t>
+Compartments, Groups, Policies will be created in Home Region So while executing setUpOCI, Enter Region as your tenancy's Home Region for Compartment Creation</t>
+  </si>
+  <si>
+    <t># Rows after &lt;END&gt; or &lt;end&gt; will not be processed;
+Group Name is mandatory field
+Enter Region as your tenancy's Home Region for Group Creation</t>
+  </si>
+  <si>
+    <t>$ and * in PolicyStatements would be replaced by PolicyStatementGroup and PolicyStatementCompartment respectively;
+# Rows after &lt;END&gt; or &lt;end&gt; will not be processed;
+Enter Region as your tenancy's Home Region for Policy Creation</t>
   </si>
 </sst>
 </file>
@@ -913,7 +915,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1019,6 +1021,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1064,17 +1075,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1115,6 +1117,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1419,99 +1426,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="18"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>204</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>205</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="40"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="D2" s="13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>97</v>
-      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1522,7 +1547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
@@ -1535,24 +1560,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="18" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
-        <v>207</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="A1" s="39" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>49</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>50</v>
@@ -1565,10 +1590,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="35" t="s">
         <v>53</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -1585,8 +1610,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
-      <c r="B4" s="39"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="9" t="s">
         <v>58</v>
       </c>
@@ -1601,10 +1626,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
-      <c r="B5" s="39"/>
+      <c r="A5" s="38"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>62</v>
@@ -1617,8 +1642,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
-      <c r="B6" s="39"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="10"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
@@ -1629,8 +1654,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
-      <c r="B7" s="39"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="12"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
@@ -1639,8 +1664,8 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
-      <c r="B8" s="39"/>
+      <c r="A8" s="38"/>
+      <c r="B8" s="36"/>
       <c r="C8" s="12"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
@@ -1649,8 +1674,8 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
-      <c r="B9" s="39"/>
+      <c r="A9" s="38"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="12"/>
       <c r="D9" s="1"/>
       <c r="E9" s="11" t="s">
@@ -1659,8 +1684,8 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
-      <c r="B10" s="39"/>
+      <c r="A10" s="38"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="12"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
@@ -1669,8 +1694,8 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
-      <c r="B11" s="39"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="12"/>
       <c r="D11" s="1"/>
       <c r="E11" s="11" t="s">
@@ -1679,8 +1704,8 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
-      <c r="B12" s="39"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="36"/>
       <c r="C12" s="12"/>
       <c r="D12" s="1"/>
       <c r="E12" s="11" t="s">
@@ -1689,8 +1714,8 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
-      <c r="B13" s="39"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="12"/>
       <c r="D13" s="1"/>
       <c r="E13" s="11" t="s">
@@ -1699,8 +1724,8 @@
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
-      <c r="B14" s="39"/>
+      <c r="A14" s="38"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="12"/>
       <c r="D14" s="1"/>
       <c r="E14" s="11" t="s">
@@ -1709,8 +1734,8 @@
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
-      <c r="B15" s="39"/>
+      <c r="A15" s="38"/>
+      <c r="B15" s="36"/>
       <c r="C15" s="10"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
@@ -1719,8 +1744,8 @@
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
-      <c r="B16" s="39"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="36"/>
       <c r="C16" s="10"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
@@ -1729,8 +1754,8 @@
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
-      <c r="B17" s="39"/>
+      <c r="A17" s="38"/>
+      <c r="B17" s="36"/>
       <c r="C17" s="10"/>
       <c r="D17" s="1"/>
       <c r="E17" s="11" t="s">
@@ -1739,8 +1764,8 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="38"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="10"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
@@ -1785,24 +1810,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="18" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
-        <v>168</v>
-      </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
+      <c r="A1" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>77</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>50</v>
@@ -1816,42 +1841,42 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B3" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>147</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C4" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="E4" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="D4" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>166</v>
-      </c>
       <c r="F4" s="16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1881,24 +1906,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="18" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
-        <v>169</v>
-      </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
+      <c r="A1" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D2" s="19" t="s">
         <v>50</v>
@@ -1912,42 +1937,42 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C4" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="E4" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>166</v>
-      </c>
       <c r="F4" s="18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1963,7 +1988,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1980,41 +2005,41 @@
     <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
-        <v>184</v>
-      </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
+    <row r="1" spans="1:10" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E2" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="13" t="s">
         <v>117</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>119</v>
       </c>
       <c r="H2" s="13"/>
       <c r="I2" s="21"/>
@@ -2022,7 +2047,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2030,13 +2055,13 @@
         <v>63</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -2044,7 +2069,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2052,13 +2077,13 @@
         <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -2112,74 +2137,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
-        <v>201</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
+      <c r="A1" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D2" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="G2" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="H2" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="I2" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="J2" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="K2" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="L2" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="M2" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="N2" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="O2" s="13" t="s">
         <v>135</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2187,16 +2212,16 @@
         <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G3" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -2212,24 +2237,24 @@
     </row>
     <row r="4" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G4" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -2241,7 +2266,7 @@
     </row>
     <row r="5" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2249,10 +2274,10 @@
         <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G5" s="1" t="b">
         <v>0</v>
@@ -2261,7 +2286,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -2346,25 +2371,25 @@
   <sheetData>
     <row r="1" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E1" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>117</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>119</v>
       </c>
       <c r="H1" s="13"/>
       <c r="I1" s="21"/>
@@ -2399,49 +2424,49 @@
   <sheetData>
     <row r="1" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D1" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="M1" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>135</v>
-      </c>
-      <c r="N1" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>137</v>
       </c>
       <c r="P1" s="13"/>
       <c r="Q1" s="21"/>
@@ -2484,69 +2509,84 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="18"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="B1" s="27"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="40"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="13" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2555,131 +2595,145 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="18"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="29"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="41" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="G2" s="42" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
-        <v>142</v>
-      </c>
+      <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="E6" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
-        <v>108</v>
-      </c>
+      <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>96</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2710,25 +2764,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
-        <v>205</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="32"/>
+      <c r="A1" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="29"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -2761,21 +2815,21 @@
         <v>11</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>26</v>
@@ -2805,12 +2859,12 @@
         <v>89</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>30</v>
@@ -2849,13 +2903,13 @@
     </row>
     <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>186</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>189</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>26</v>
@@ -2870,7 +2924,7 @@
         <v>26</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I5" s="3">
         <v>2</v>
@@ -2885,7 +2939,7 @@
         <v>89</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2956,48 +3010,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="181.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="B1" s="34"/>
+      <c r="A1" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" s="31"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>27</v>
@@ -3005,7 +3059,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>26</v>
@@ -3013,32 +3067,32 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
-        <v>196</v>
-      </c>
-      <c r="B10" s="36"/>
+      <c r="A10" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="B10" s="33"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -3075,23 +3129,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
+      <c r="A1" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
     </row>
     <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -3121,7 +3175,7 @@
         <v>47</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -3135,7 +3189,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
@@ -3156,7 +3210,7 @@
         <v>27</v>
       </c>
       <c r="K3" s="20" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -3240,13 +3294,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
-        <v>195</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
+      <c r="A1" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
     </row>
     <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3336,24 +3390,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
-        <v>160</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="32"/>
+      <c r="A1" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="29"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>77</v>
@@ -3383,18 +3437,18 @@
         <v>85</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>
@@ -3412,7 +3466,7 @@
         <v>18</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>19</v>
@@ -3424,7 +3478,7 @@
         <v>91</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -3471,20 +3525,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="18" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
-        <v>159</v>
-      </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
+      <c r="A1" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>37</v>
@@ -3502,18 +3556,18 @@
         <v>41</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C3" s="1">
         <v>302</v>
@@ -3522,7 +3576,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>16</v>
@@ -3531,7 +3585,7 @@
         <v>91</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>